<commit_message>
new pdf of Rmd
</commit_message>
<xml_diff>
--- a/data/derived/arc-storage-t1-flux/arc-inc_xplr_arc-storage-t1-flux_2020-04-27.xlsx
+++ b/data/derived/arc-storage-t1-flux/arc-inc_xplr_arc-storage-t1-flux_2020-04-27.xlsx
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4197" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4185" uniqueCount="446">
   <si>
     <t>Site</t>
   </si>
@@ -1446,9 +1446,6 @@
     <t>Experiment</t>
   </si>
   <si>
-    <t>arc</t>
-  </si>
-  <si>
     <t>tme</t>
   </si>
 </sst>
@@ -1616,18 +1613,7 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
@@ -55842,8 +55828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -55936,8 +55922,8 @@
       </c>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="2" t="s">
-        <v>445</v>
+      <c r="A2" s="2">
+        <v>2011</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>187</v>
@@ -56020,8 +56006,8 @@
       </c>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="2" t="s">
-        <v>445</v>
+      <c r="A3" s="2">
+        <v>2011</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>211</v>
@@ -56104,8 +56090,8 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="2" t="s">
-        <v>445</v>
+      <c r="A4" s="2">
+        <v>2011</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>227</v>
@@ -56188,8 +56174,8 @@
       </c>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="2" t="s">
-        <v>445</v>
+      <c r="A5" s="2">
+        <v>2011</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>253</v>
@@ -56272,8 +56258,8 @@
       </c>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="2" t="s">
-        <v>445</v>
+      <c r="A6" s="2">
+        <v>2011</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>275</v>
@@ -56356,8 +56342,8 @@
       </c>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="2" t="s">
-        <v>445</v>
+      <c r="A7" s="2">
+        <v>2011</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>274</v>
@@ -56440,8 +56426,8 @@
       </c>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="2" t="s">
-        <v>445</v>
+      <c r="A8" s="2">
+        <v>2011</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>326</v>
@@ -56524,8 +56510,8 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="2" t="s">
-        <v>445</v>
+      <c r="A9" s="2">
+        <v>2011</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>328</v>
@@ -56608,8 +56594,8 @@
       </c>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="2" t="s">
-        <v>445</v>
+      <c r="A10" s="2">
+        <v>2011</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>334</v>
@@ -56692,8 +56678,8 @@
       </c>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="2" t="s">
-        <v>445</v>
+      <c r="A11" s="2">
+        <v>2011</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>351</v>
@@ -56776,8 +56762,8 @@
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="2" t="s">
-        <v>445</v>
+      <c r="A12" s="2">
+        <v>2011</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>374</v>
@@ -56860,8 +56846,8 @@
       </c>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="2" t="s">
-        <v>445</v>
+      <c r="A13" s="2">
+        <v>2011</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>383</v>
@@ -56945,7 +56931,7 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>257</v>
@@ -57029,7 +57015,7 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>280</v>
@@ -57113,7 +57099,7 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>197</v>
@@ -57197,7 +57183,7 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>212</v>
@@ -57281,7 +57267,7 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>183</v>
@@ -57365,7 +57351,7 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>282</v>

</xml_diff>